<commit_message>
I added a distance column
</commit_message>
<xml_diff>
--- a/public/v1/Wisconsin State Parks.xlsx
+++ b/public/v1/Wisconsin State Parks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joe/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joe/Code/WIStateParks-API/public/v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E70B051-E940-1048-95E8-4593F005AF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B334148C-E540-9B46-A655-38489B64CE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="500" windowWidth="16980" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="697">
   <si>
     <t>name</t>
   </si>
@@ -2177,6 +2177,9 @@
   </si>
   <si>
     <t>LatLongCoordinates</t>
+  </si>
+  <si>
+    <t>distance</t>
   </si>
 </sst>
 </file>
@@ -2463,13 +2466,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2:N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2485,7 +2488,7 @@
     <col min="13" max="13" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2525,8 +2528,11 @@
       <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N1" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2566,8 +2572,11 @@
       <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2607,8 +2616,11 @@
       <c r="M3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2648,8 +2660,11 @@
       <c r="M4" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -2689,8 +2704,11 @@
       <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -2730,8 +2748,11 @@
       <c r="M6" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -2771,8 +2792,11 @@
       <c r="M7" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
@@ -2812,8 +2836,11 @@
       <c r="M8" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -2853,8 +2880,11 @@
       <c r="M9" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -2894,8 +2924,11 @@
       <c r="M10" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>93</v>
       </c>
@@ -2935,8 +2968,11 @@
       <c r="M11" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>102</v>
       </c>
@@ -2976,8 +3012,11 @@
       <c r="M12" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -3017,8 +3056,11 @@
       <c r="M13" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>121</v>
       </c>
@@ -3058,8 +3100,11 @@
       <c r="M14" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>131</v>
       </c>
@@ -3099,8 +3144,11 @@
       <c r="M15" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>141</v>
       </c>
@@ -3140,8 +3188,11 @@
       <c r="M16" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>151</v>
       </c>
@@ -3181,8 +3232,11 @@
       <c r="M17" s="6" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -3222,8 +3276,11 @@
       <c r="M18" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>169</v>
       </c>
@@ -3263,8 +3320,11 @@
       <c r="M19" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>178</v>
       </c>
@@ -3304,8 +3364,11 @@
       <c r="M20" s="6" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>187</v>
       </c>
@@ -3345,8 +3408,11 @@
       <c r="M21" s="6" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>196</v>
       </c>
@@ -3386,8 +3452,11 @@
       <c r="M22" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>206</v>
       </c>
@@ -3427,8 +3496,11 @@
       <c r="M23" s="6" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>214</v>
       </c>
@@ -3468,8 +3540,11 @@
       <c r="M24" s="6" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>224</v>
       </c>
@@ -3509,8 +3584,11 @@
       <c r="M25" s="6" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>233</v>
       </c>
@@ -3550,8 +3628,11 @@
       <c r="M26" s="6" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>241</v>
       </c>
@@ -3591,8 +3672,11 @@
       <c r="M27" s="6" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>251</v>
       </c>
@@ -3632,8 +3716,11 @@
       <c r="M28" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>261</v>
       </c>
@@ -3673,8 +3760,11 @@
       <c r="M29" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>270</v>
       </c>
@@ -3714,8 +3804,11 @@
       <c r="M30" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>280</v>
       </c>
@@ -3755,8 +3848,11 @@
       <c r="M31" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>290</v>
       </c>
@@ -3796,8 +3892,11 @@
       <c r="M32" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>299</v>
       </c>
@@ -3837,8 +3936,11 @@
       <c r="M33" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>309</v>
       </c>
@@ -3878,8 +3980,11 @@
       <c r="M34" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>319</v>
       </c>
@@ -3919,8 +4024,11 @@
       <c r="M35" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>329</v>
       </c>
@@ -3960,8 +4068,11 @@
       <c r="M36" s="1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>339</v>
       </c>
@@ -4001,8 +4112,11 @@
       <c r="M37" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>348</v>
       </c>
@@ -4042,8 +4156,11 @@
       <c r="M38" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>358</v>
       </c>
@@ -4083,8 +4200,11 @@
       <c r="M39" s="1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N39">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>366</v>
       </c>
@@ -4124,8 +4244,11 @@
       <c r="M40" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>375</v>
       </c>
@@ -4165,8 +4288,11 @@
       <c r="M41" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>384</v>
       </c>
@@ -4206,8 +4332,11 @@
       <c r="M42" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>393</v>
       </c>
@@ -4247,8 +4376,11 @@
       <c r="M43" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N43">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>400</v>
       </c>
@@ -4288,8 +4420,11 @@
       <c r="M44" s="1" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>408</v>
       </c>
@@ -4329,8 +4464,11 @@
       <c r="M45" s="1" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>417</v>
       </c>
@@ -4370,8 +4508,11 @@
       <c r="M46" s="1" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>425</v>
       </c>
@@ -4411,8 +4552,11 @@
       <c r="M47" s="1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N47">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>433</v>
       </c>
@@ -4452,8 +4596,11 @@
       <c r="M48" s="6" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N48">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>443</v>
       </c>
@@ -4493,8 +4640,11 @@
       <c r="M49" s="6" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N49">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>451</v>
       </c>
@@ -4534,8 +4684,11 @@
       <c r="M50" s="6" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N50">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>460</v>
       </c>
@@ -4575,8 +4728,11 @@
       <c r="M51" s="6" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N51">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>469</v>
       </c>
@@ -4616,8 +4772,11 @@
       <c r="M52" s="6" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N52">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>478</v>
       </c>
@@ -4657,8 +4816,11 @@
       <c r="M53" s="6" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>485</v>
       </c>
@@ -4698,8 +4860,11 @@
       <c r="M54" s="6" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N54">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>494</v>
       </c>
@@ -4739,8 +4904,11 @@
       <c r="M55" s="6" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>501</v>
       </c>
@@ -4780,8 +4948,11 @@
       <c r="M56" s="6" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>511</v>
       </c>
@@ -4821,8 +4992,11 @@
       <c r="M57" s="6" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>521</v>
       </c>
@@ -4862,8 +5036,11 @@
       <c r="M58" s="6" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N58">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>530</v>
       </c>
@@ -4903,8 +5080,11 @@
       <c r="M59" s="6" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>538</v>
       </c>
@@ -4944,8 +5124,11 @@
       <c r="M60" s="6" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N60">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>547</v>
       </c>
@@ -4985,8 +5168,11 @@
       <c r="M61" s="6" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N61">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>554</v>
       </c>
@@ -5026,8 +5212,11 @@
       <c r="M62" s="6" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>562</v>
       </c>
@@ -5067,8 +5256,11 @@
       <c r="M63" s="6" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N63">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>570</v>
       </c>
@@ -5108,8 +5300,11 @@
       <c r="M64" s="6" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N64">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>579</v>
       </c>
@@ -5149,8 +5344,11 @@
       <c r="M65" s="6" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N65">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>589</v>
       </c>
@@ -5190,8 +5388,11 @@
       <c r="M66" s="6" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N66">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>598</v>
       </c>
@@ -5231,8 +5432,11 @@
       <c r="M67" s="6" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N67">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>607</v>
       </c>
@@ -5272,8 +5476,11 @@
       <c r="M68" s="6" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N68">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>615</v>
       </c>
@@ -5313,8 +5520,11 @@
       <c r="M69" s="6" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>623</v>
       </c>
@@ -5354,8 +5564,11 @@
       <c r="M70" s="6" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N70">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>630</v>
       </c>
@@ -5395,8 +5608,11 @@
       <c r="M71" s="6" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N71">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>638</v>
       </c>
@@ -5436,8 +5652,11 @@
       <c r="M72" s="6" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>648</v>
       </c>
@@ -5477,8 +5696,11 @@
       <c r="M73" s="6" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N73">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>657</v>
       </c>
@@ -5518,8 +5740,11 @@
       <c r="M74" s="6" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N74">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>665</v>
       </c>
@@ -5559,8 +5784,11 @@
       <c r="M75" s="6" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N75">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>673</v>
       </c>
@@ -5600,8 +5828,11 @@
       <c r="M76" s="6" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="N76">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>681</v>
       </c>
@@ -5640,6 +5871,9 @@
       </c>
       <c r="M77" s="6" t="s">
         <v>688</v>
+      </c>
+      <c r="N77">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>